<commit_message>
Versão com variáveis, histórico de data e busca combinada
</commit_message>
<xml_diff>
--- a/lista_consolidada.xlsx
+++ b/lista_consolidada.xlsx
@@ -40,19 +40,19 @@
     <t xml:space="preserve">Preço da Quantidade Sugerida</t>
   </si>
   <si>
-    <t xml:space="preserve">Agulha</t>
+    <t xml:space="preserve">Agulha de talagarça</t>
   </si>
   <si>
     <t xml:space="preserve">Para talagarça</t>
   </si>
   <si>
-    <t xml:space="preserve">Agenda</t>
+    <t xml:space="preserve">Agenda escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Escolar (2026)</t>
   </si>
   <si>
-    <t xml:space="preserve">Apontador</t>
+    <t xml:space="preserve">Apontador escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Com depósito/reservatório</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">A3 (Branco, 140g ou 200g)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bloco Criativo</t>
+    <t xml:space="preserve">Bloco Criativo papel colorido A4</t>
   </si>
   <si>
     <t xml:space="preserve">Papel colorido A4</t>
@@ -73,13 +73,13 @@
     <t xml:space="preserve">Pacote</t>
   </si>
   <si>
-    <t xml:space="preserve">Borracha</t>
+    <t xml:space="preserve">Borracha escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Branca simples</t>
   </si>
   <si>
-    <t xml:space="preserve">Caderno</t>
+    <t xml:space="preserve">Caderno de desenho</t>
   </si>
   <si>
     <t xml:space="preserve">Desenho espiral/brochura (48 fls)</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Conjunto</t>
   </si>
   <si>
-    <t xml:space="preserve">Cartolina</t>
+    <t xml:space="preserve">Cartolina folha</t>
   </si>
   <si>
     <t xml:space="preserve">Branca ou cores variadas</t>
@@ -103,19 +103,19 @@
     <t xml:space="preserve">Folha</t>
   </si>
   <si>
-    <t xml:space="preserve">Cola Bastão</t>
+    <t xml:space="preserve">Cola Bastão escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Tamanho médio</t>
   </si>
   <si>
-    <t xml:space="preserve">Cola Branca</t>
+    <t xml:space="preserve">Cola Branca escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Tubo (110g ou 500g)</t>
   </si>
   <si>
-    <t xml:space="preserve">Estojo</t>
+    <t xml:space="preserve">Estojo escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Com divisões</t>
@@ -130,19 +130,19 @@
     <t xml:space="preserve">Caixa</t>
   </si>
   <si>
-    <t xml:space="preserve">Lápis de Cor</t>
+    <t xml:space="preserve">Lápis de Cor caixa 12 ou 24 cores</t>
   </si>
   <si>
     <t xml:space="preserve">12 ou 24 cores</t>
   </si>
   <si>
-    <t xml:space="preserve">Lápis Preto</t>
+    <t xml:space="preserve">Lápis Preto n 2</t>
   </si>
   <si>
     <t xml:space="preserve">Tipo HB ou 2B (Triangular)</t>
   </si>
   <si>
-    <t xml:space="preserve">Massa de Modelar</t>
+    <t xml:space="preserve">Massa de Modelar escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Pote de 500g ou amido</t>
@@ -151,37 +151,37 @@
     <t xml:space="preserve">Pote/Caixa</t>
   </si>
   <si>
-    <t xml:space="preserve">Papel A4</t>
+    <t xml:space="preserve">Papel A4 pacote</t>
   </si>
   <si>
     <t xml:space="preserve">Sulfite branco (100 fls)</t>
   </si>
   <si>
-    <t xml:space="preserve">Pasta</t>
+    <t xml:space="preserve">Pasta escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Plástica com elástico A4</t>
   </si>
   <si>
-    <t xml:space="preserve">Régua</t>
+    <t xml:space="preserve">Régua escolar</t>
   </si>
   <si>
     <t xml:space="preserve">30 cm</t>
   </si>
   <si>
-    <t xml:space="preserve">Tesoura</t>
+    <t xml:space="preserve">Tesoura escolar</t>
   </si>
   <si>
     <t xml:space="preserve">Pequena sem ponta</t>
   </si>
   <si>
-    <t xml:space="preserve">Tinta Guache</t>
+    <t xml:space="preserve">Tinta Guache pote 250 gr</t>
   </si>
   <si>
     <t xml:space="preserve">Potes de cores variadas (250g)</t>
   </si>
   <si>
-    <t xml:space="preserve">TNT</t>
+    <t xml:space="preserve">TNT metro</t>
   </si>
   <si>
     <t xml:space="preserve">Cores variadas</t>
@@ -197,7 +197,7 @@
     <t xml:space="preserve">unidade</t>
   </si>
   <si>
-    <t xml:space="preserve">Pincel</t>
+    <t xml:space="preserve">Pincel n 10 </t>
   </si>
   <si>
     <t xml:space="preserve">Nº 10 ou batedor de espuma 
@@ -616,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Otimização e simplificação da tabela lista_consolidada e exclusão da tabela lista_com_melhores_precos.xlsx
</commit_message>
<xml_diff>
--- a/lista_consolidada.xlsx
+++ b/lista_consolidada.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -43,31 +43,31 @@
     <t xml:space="preserve">Agulha de talagarça</t>
   </si>
   <si>
-    <t xml:space="preserve">Para talagarça</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agenda escolar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escolar (2026)</t>
+    <t xml:space="preserve">Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agenda escolar 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capa dura</t>
   </si>
   <si>
     <t xml:space="preserve">Apontador escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Com depósito/reservatório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloco de Desenho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A3 (Branco, 140g ou 200g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloco Criativo papel colorido A4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papel colorido A4</t>
+    <t xml:space="preserve">Com depósito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloco de Desenho A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branco 140g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloco Papel Criativo A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorido</t>
   </si>
   <si>
     <t xml:space="preserve">Pacote</t>
@@ -76,19 +76,19 @@
     <t xml:space="preserve">Borracha escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Branca simples</t>
+    <t xml:space="preserve">Branca</t>
   </si>
   <si>
     <t xml:space="preserve">Caderno de desenho</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenho espiral/brochura (48 fls)</t>
+    <t xml:space="preserve">Espiral 48 fls</t>
   </si>
   <si>
     <t xml:space="preserve">Canetinha Hidrocor</t>
   </si>
   <si>
-    <t xml:space="preserve">Conjunto com 12 cores</t>
+    <t xml:space="preserve">12 cores</t>
   </si>
   <si>
     <t xml:space="preserve">Conjunto</t>
@@ -97,70 +97,76 @@
     <t xml:space="preserve">Cartolina folha</t>
   </si>
   <si>
-    <t xml:space="preserve">Branca ou cores variadas</t>
+    <t xml:space="preserve">Cores variadas</t>
   </si>
   <si>
     <t xml:space="preserve">Folha</t>
   </si>
   <si>
-    <t xml:space="preserve">Cola Bastão escolar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamanho médio</t>
+    <t xml:space="preserve">Cola Bastão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20g</t>
   </si>
   <si>
     <t xml:space="preserve">Cola Branca escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubo (110g ou 500g)</t>
+    <t xml:space="preserve">110g</t>
   </si>
   <si>
     <t xml:space="preserve">Estojo escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Com divisões</t>
+    <t xml:space="preserve">com divisória</t>
   </si>
   <si>
     <t xml:space="preserve">Giz de Cera</t>
   </si>
   <si>
-    <t xml:space="preserve">12 cores (Jumbo ou Comum)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Caixa</t>
   </si>
   <si>
-    <t xml:space="preserve">Lápis de Cor caixa 12 ou 24 cores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 ou 24 cores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lápis Preto n 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo HB ou 2B (Triangular)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Massa de Modelar escolar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pote de 500g ou amido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pote/Caixa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papel A4 pacote</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulfite branco (100 fls)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasta escolar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plástica com elástico A4</t>
+    <t xml:space="preserve">Lápis de Cor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 cores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lápis Preto HB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n 2 Triangular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massa de Modelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pote 500g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papel A4 Sulfite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 folhas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasta escolar A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com elástico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com aba e elástico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pincel n 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chato ou Redondo</t>
   </si>
   <si>
     <t xml:space="preserve">Régua escolar</t>
@@ -169,65 +175,31 @@
     <t xml:space="preserve">30 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">Tela de Pintura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20x30 ou 30x40</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tesoura escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Pequena sem ponta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tinta Guache pote 250 gr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potes de cores variadas (250g)</t>
+    <t xml:space="preserve">sem ponta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tinta Guache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pote 250g</t>
   </si>
   <si>
     <t xml:space="preserve">TNT metro</t>
   </si>
   <si>
-    <t xml:space="preserve">Cores variadas</t>
+    <t xml:space="preserve">Branco ou cores</t>
   </si>
   <si>
     <t xml:space="preserve">Metro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plástica com aba e elástico A4 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pincel n 10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nº 10 ou batedor de espuma 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 cm 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela de Pintura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamanhos diversos (20x30 a 30x40) 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pequena sem ponta 
-+2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pote de 250g (Cores variadas) 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branco ou cores variadas (metro) 
-+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metro</t>
   </si>
 </sst>
 </file>
@@ -237,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -271,14 +243,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="&quot;Google Sans Text&quot;"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -332,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,20 +313,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -445,37 +401,37 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285f4"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ea4335"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="fbbc04"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34a853"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="ff6d01"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46bdc6"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -616,11 +572,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.2"/>
@@ -654,13 +610,13 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
@@ -670,13 +626,13 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="n">
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="5"/>
@@ -686,13 +642,13 @@
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="n">
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
@@ -702,13 +658,13 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="5"/>
@@ -718,13 +674,13 @@
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="5"/>
@@ -734,13 +690,13 @@
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="n">
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="5"/>
@@ -750,13 +706,13 @@
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="5"/>
@@ -766,13 +722,13 @@
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="5"/>
@@ -782,13 +738,13 @@
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="5"/>
@@ -798,13 +754,13 @@
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="n">
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="5"/>
@@ -814,13 +770,13 @@
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="n">
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="5"/>
@@ -830,13 +786,13 @@
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="n">
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="5"/>
@@ -846,13 +802,13 @@
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="5"/>
@@ -860,15 +816,15 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2" t="n">
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="5"/>
@@ -876,15 +832,15 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="n">
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E16" s="5"/>
@@ -892,15 +848,15 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="5"/>
@@ -908,15 +864,15 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="5"/>
@@ -924,15 +880,15 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="n">
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="5"/>
@@ -940,15 +896,15 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="5"/>
@@ -956,15 +912,15 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="5"/>
@@ -972,148 +928,88 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>1</v>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>1</v>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="7" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="2" t="n">
-        <v>1</v>
+      <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>